<commit_message>
Cleaned Film Names And Added Movie Selection Reactive Output
</commit_message>
<xml_diff>
--- a/FandangoLovesMovies/movie_ratings.xlsx
+++ b/FandangoLovesMovies/movie_ratings.xlsx
@@ -397,7 +397,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Avengers: Age of Ultron (2015)</t>
+          <t xml:space="preserve">Avengers: Age of Ultron </t>
         </is>
       </c>
       <c r="B2">
@@ -422,7 +422,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cinderella (2015)</t>
+          <t xml:space="preserve">Cinderella </t>
         </is>
       </c>
       <c r="B3">
@@ -447,7 +447,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ant-Man (2015)</t>
+          <t xml:space="preserve">Ant-Man </t>
         </is>
       </c>
       <c r="B4">
@@ -472,7 +472,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Do You Believe? (2015)</t>
+          <t xml:space="preserve">Do You Believe? </t>
         </is>
       </c>
       <c r="B5">
@@ -497,7 +497,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Hot Tub Time Machine 2 (2015)</t>
+          <t xml:space="preserve">Hot Tub Time Machine 2 </t>
         </is>
       </c>
       <c r="B6">
@@ -522,7 +522,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>The Water Diviner (2015)</t>
+          <t xml:space="preserve">The Water Diviner </t>
         </is>
       </c>
       <c r="B7">
@@ -547,7 +547,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Top Five (2014)</t>
+          <t xml:space="preserve">Top Five </t>
         </is>
       </c>
       <c r="B8">
@@ -572,7 +572,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Shaun the Sheep Movie (2015)</t>
+          <t xml:space="preserve">Shaun the Sheep Movie </t>
         </is>
       </c>
       <c r="B9">
@@ -597,7 +597,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Love &amp; Mercy (2015)</t>
+          <t xml:space="preserve">Love &amp; Mercy </t>
         </is>
       </c>
       <c r="B10">
@@ -622,7 +622,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Far From The Madding Crowd (2015)</t>
+          <t xml:space="preserve">Far From The Madding Crowd </t>
         </is>
       </c>
       <c r="B11">
@@ -647,7 +647,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Black Sea (2015)</t>
+          <t xml:space="preserve">Black Sea </t>
         </is>
       </c>
       <c r="B12">
@@ -672,7 +672,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Leviathan (2014)</t>
+          <t xml:space="preserve">Leviathan </t>
         </is>
       </c>
       <c r="B13">
@@ -697,7 +697,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Unbroken (2014)</t>
+          <t xml:space="preserve">Unbroken </t>
         </is>
       </c>
       <c r="B14">
@@ -722,7 +722,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>The Imitation Game (2014)</t>
+          <t xml:space="preserve">The Imitation Game </t>
         </is>
       </c>
       <c r="B15">
@@ -747,7 +747,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Taken 3 (2015)</t>
+          <t xml:space="preserve">Taken 3 </t>
         </is>
       </c>
       <c r="B16">
@@ -772,7 +772,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ted 2 (2015)</t>
+          <t xml:space="preserve">Ted 2 </t>
         </is>
       </c>
       <c r="B17">
@@ -797,7 +797,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Southpaw (2015)</t>
+          <t xml:space="preserve">Southpaw </t>
         </is>
       </c>
       <c r="B18">
@@ -822,7 +822,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Night at the Museum: Secret of the Tomb (2014)</t>
+          <t xml:space="preserve">Night at the Museum: Secret of the Tomb </t>
         </is>
       </c>
       <c r="B19">
@@ -847,7 +847,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Pixels (2015)</t>
+          <t xml:space="preserve">Pixels </t>
         </is>
       </c>
       <c r="B20">
@@ -872,7 +872,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>McFarland, USA (2015)</t>
+          <t xml:space="preserve">McFarland, USA </t>
         </is>
       </c>
       <c r="B21">
@@ -897,7 +897,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Insidious: Chapter 3 (2015)</t>
+          <t xml:space="preserve">Insidious: Chapter 3 </t>
         </is>
       </c>
       <c r="B22">
@@ -922,7 +922,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>The Man From U.N.C.L.E. (2015)</t>
+          <t xml:space="preserve">The Man From U.N.C.L.E. </t>
         </is>
       </c>
       <c r="B23">
@@ -947,7 +947,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Run All Night (2015)</t>
+          <t xml:space="preserve">Run All Night </t>
         </is>
       </c>
       <c r="B24">
@@ -972,7 +972,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Trainwreck (2015)</t>
+          <t xml:space="preserve">Trainwreck </t>
         </is>
       </c>
       <c r="B25">
@@ -997,7 +997,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Selma (2014)</t>
+          <t xml:space="preserve">Selma </t>
         </is>
       </c>
       <c r="B26">
@@ -1022,7 +1022,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Ex Machina (2015)</t>
+          <t xml:space="preserve">Ex Machina </t>
         </is>
       </c>
       <c r="B27">
@@ -1047,7 +1047,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Still Alice (2015)</t>
+          <t xml:space="preserve">Still Alice </t>
         </is>
       </c>
       <c r="B28">
@@ -1072,7 +1072,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Wild Tales (2014)</t>
+          <t xml:space="preserve">Wild Tales </t>
         </is>
       </c>
       <c r="B29">
@@ -1097,7 +1097,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>The Boy Next Door (2015)</t>
+          <t xml:space="preserve">The Boy Next Door </t>
         </is>
       </c>
       <c r="B30">
@@ -1122,7 +1122,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Aloha (2015)</t>
+          <t xml:space="preserve">Aloha </t>
         </is>
       </c>
       <c r="B31">
@@ -1147,7 +1147,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>The Loft (2015)</t>
+          <t xml:space="preserve">The Loft </t>
         </is>
       </c>
       <c r="B32">
@@ -1172,7 +1172,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Welcome to Me (2015)</t>
+          <t xml:space="preserve">Welcome to Me </t>
         </is>
       </c>
       <c r="B33">
@@ -1197,7 +1197,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Maps to the Stars (2015)</t>
+          <t xml:space="preserve">Maps to the Stars </t>
         </is>
       </c>
       <c r="B34">
@@ -1222,7 +1222,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Timbuktu (2015)</t>
+          <t xml:space="preserve">Timbuktu </t>
         </is>
       </c>
       <c r="B35">
@@ -1247,7 +1247,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Kingsman: The Secret Service (2015)</t>
+          <t xml:space="preserve">Kingsman: The Secret Service </t>
         </is>
       </c>
       <c r="B36">
@@ -1272,7 +1272,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Tomorrowland (2015)</t>
+          <t xml:space="preserve">Tomorrowland </t>
         </is>
       </c>
       <c r="B37">
@@ -1297,7 +1297,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>The Divergent Series: Insurgent (2015)</t>
+          <t xml:space="preserve">The Divergent Series: Insurgent </t>
         </is>
       </c>
       <c r="B38">
@@ -1322,7 +1322,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Annie (2014)</t>
+          <t xml:space="preserve">Annie </t>
         </is>
       </c>
       <c r="B39">
@@ -1347,7 +1347,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Fantastic Four (2015)</t>
+          <t xml:space="preserve">Fantastic Four </t>
         </is>
       </c>
       <c r="B40">
@@ -1372,7 +1372,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Terminator Genisys (2015)</t>
+          <t xml:space="preserve">Terminator Genisys </t>
         </is>
       </c>
       <c r="B41">
@@ -1397,7 +1397,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Pitch Perfect 2 (2015)</t>
+          <t xml:space="preserve">Pitch Perfect 2 </t>
         </is>
       </c>
       <c r="B42">
@@ -1422,7 +1422,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Entourage (2015)</t>
+          <t xml:space="preserve">Entourage </t>
         </is>
       </c>
       <c r="B43">
@@ -1447,7 +1447,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>The Age of Adaline (2015)</t>
+          <t xml:space="preserve">The Age of Adaline </t>
         </is>
       </c>
       <c r="B44">
@@ -1472,7 +1472,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Hot Pursuit (2015)</t>
+          <t xml:space="preserve">Hot Pursuit </t>
         </is>
       </c>
       <c r="B45">
@@ -1497,7 +1497,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>The DUFF (2015)</t>
+          <t xml:space="preserve">The DUFF </t>
         </is>
       </c>
       <c r="B46">
@@ -1522,7 +1522,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Project Almanac (2015)</t>
+          <t xml:space="preserve">Project Almanac </t>
         </is>
       </c>
       <c r="B47">
@@ -1547,7 +1547,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Ricki and the Flash (2015)</t>
+          <t xml:space="preserve">Ricki and the Flash </t>
         </is>
       </c>
       <c r="B48">
@@ -1572,7 +1572,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Seventh Son (2015)</t>
+          <t xml:space="preserve">Seventh Son </t>
         </is>
       </c>
       <c r="B49">
@@ -1597,7 +1597,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Mortdecai (2015)</t>
+          <t xml:space="preserve">Mortdecai </t>
         </is>
       </c>
       <c r="B50">
@@ -1622,7 +1622,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Unfinished Business (2015)</t>
+          <t xml:space="preserve">Unfinished Business </t>
         </is>
       </c>
       <c r="B51">
@@ -1647,7 +1647,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>American Ultra (2015)</t>
+          <t xml:space="preserve">American Ultra </t>
         </is>
       </c>
       <c r="B52">
@@ -1672,7 +1672,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>True Story (2015)</t>
+          <t xml:space="preserve">True Story </t>
         </is>
       </c>
       <c r="B53">
@@ -1697,7 +1697,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Child 44 (2015)</t>
+          <t xml:space="preserve">Child 44 </t>
         </is>
       </c>
       <c r="B54">
@@ -1722,7 +1722,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Birdman (2014)</t>
+          <t xml:space="preserve">Birdman </t>
         </is>
       </c>
       <c r="B55">
@@ -1747,7 +1747,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>The Gift (2015)</t>
+          <t xml:space="preserve">The Gift </t>
         </is>
       </c>
       <c r="B56">
@@ -1772,7 +1772,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Unfriended (2015)</t>
+          <t xml:space="preserve">Unfriended </t>
         </is>
       </c>
       <c r="B57">
@@ -1797,7 +1797,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Mr. Turner (2014)</t>
+          <t xml:space="preserve">Mr. Turner </t>
         </is>
       </c>
       <c r="B58">
@@ -1822,7 +1822,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>American Sniper (2015)</t>
+          <t xml:space="preserve">American Sniper </t>
         </is>
       </c>
       <c r="B59">
@@ -1847,7 +1847,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Furious 7 (2015)</t>
+          <t xml:space="preserve">Furious 7 </t>
         </is>
       </c>
       <c r="B60">
@@ -1872,7 +1872,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>The Hobbit: The Battle of the Five Armies (2014)</t>
+          <t xml:space="preserve">The Hobbit: The Battle of the Five Armies </t>
         </is>
       </c>
       <c r="B61">
@@ -1897,7 +1897,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>San Andreas (2015)</t>
+          <t xml:space="preserve">San Andreas </t>
         </is>
       </c>
       <c r="B62">
@@ -1922,7 +1922,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Straight Outta Compton (2015)</t>
+          <t xml:space="preserve">Straight Outta Compton </t>
         </is>
       </c>
       <c r="B63">
@@ -1947,7 +1947,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Vacation (2015)</t>
+          <t xml:space="preserve">Vacation </t>
         </is>
       </c>
       <c r="B64">
@@ -1972,7 +1972,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Chappie (2015)</t>
+          <t xml:space="preserve">Chappie </t>
         </is>
       </c>
       <c r="B65">
@@ -1997,7 +1997,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Poltergeist (2015)</t>
+          <t xml:space="preserve">Poltergeist </t>
         </is>
       </c>
       <c r="B66">
@@ -2022,7 +2022,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Paper Towns (2015)</t>
+          <t xml:space="preserve">Paper Towns </t>
         </is>
       </c>
       <c r="B67">
@@ -2047,7 +2047,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Big Eyes (2014)</t>
+          <t xml:space="preserve">Big Eyes </t>
         </is>
       </c>
       <c r="B68">
@@ -2072,7 +2072,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Blackhat (2015)</t>
+          <t xml:space="preserve">Blackhat </t>
         </is>
       </c>
       <c r="B69">
@@ -2097,7 +2097,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Self/less (2015)</t>
+          <t xml:space="preserve">Self/less </t>
         </is>
       </c>
       <c r="B70">
@@ -2122,7 +2122,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Sinister 2 (2015)</t>
+          <t xml:space="preserve">Sinister 2 </t>
         </is>
       </c>
       <c r="B71">
@@ -2147,7 +2147,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Little Boy (2015)</t>
+          <t xml:space="preserve">Little Boy </t>
         </is>
       </c>
       <c r="B72">
@@ -2172,7 +2172,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Me and Earl and The Dying Girl (2015)</t>
+          <t xml:space="preserve">Me and Earl and The Dying Girl </t>
         </is>
       </c>
       <c r="B73">
@@ -2197,7 +2197,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Maggie (2015)</t>
+          <t xml:space="preserve">Maggie </t>
         </is>
       </c>
       <c r="B74">
@@ -2222,7 +2222,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Mad Max: Fury Road (2015)</t>
+          <t xml:space="preserve">Mad Max: Fury Road </t>
         </is>
       </c>
       <c r="B75">
@@ -2247,7 +2247,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Spy (2015)</t>
+          <t xml:space="preserve">Spy </t>
         </is>
       </c>
       <c r="B76">
@@ -2272,7 +2272,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>The SpongeBob Movie: Sponge Out of Water (2015)</t>
+          <t xml:space="preserve">The SpongeBob Movie: Sponge Out of Water </t>
         </is>
       </c>
       <c r="B77">
@@ -2297,7 +2297,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Paddington (2015)</t>
+          <t xml:space="preserve">Paddington </t>
         </is>
       </c>
       <c r="B78">
@@ -2322,7 +2322,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Dope (2015)</t>
+          <t xml:space="preserve">Dope </t>
         </is>
       </c>
       <c r="B79">
@@ -2347,7 +2347,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>What We Do in the Shadows (2015)</t>
+          <t xml:space="preserve">What We Do in the Shadows </t>
         </is>
       </c>
       <c r="B80">
@@ -2372,7 +2372,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Song of the Sea (2014)</t>
+          <t xml:space="preserve">Song of the Sea </t>
         </is>
       </c>
       <c r="B81">
@@ -2397,7 +2397,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Fifty Shades of Grey (2015)</t>
+          <t xml:space="preserve">Fifty Shades of Grey </t>
         </is>
       </c>
       <c r="B82">
@@ -2422,7 +2422,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Get Hard (2015)</t>
+          <t xml:space="preserve">Get Hard </t>
         </is>
       </c>
       <c r="B83">
@@ -2447,7 +2447,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Focus (2015)</t>
+          <t xml:space="preserve">Focus </t>
         </is>
       </c>
       <c r="B84">
@@ -2472,7 +2472,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Jupiter Ascending (2015)</t>
+          <t xml:space="preserve">Jupiter Ascending </t>
         </is>
       </c>
       <c r="B85">
@@ -2497,7 +2497,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>The Gallows (2015)</t>
+          <t xml:space="preserve">The Gallows </t>
         </is>
       </c>
       <c r="B86">
@@ -2522,7 +2522,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>The Second Best Exotic Marigold Hotel (2015)</t>
+          <t xml:space="preserve">The Second Best Exotic Marigold Hotel </t>
         </is>
       </c>
       <c r="B87">
@@ -2547,7 +2547,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Strange Magic (2015)</t>
+          <t xml:space="preserve">Strange Magic </t>
         </is>
       </c>
       <c r="B88">
@@ -2572,7 +2572,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>The Gunman (2015)</t>
+          <t xml:space="preserve">The Gunman </t>
         </is>
       </c>
       <c r="B89">
@@ -2597,7 +2597,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Hitman: Agent 47 (2015)</t>
+          <t xml:space="preserve">Hitman: Agent 47 </t>
         </is>
       </c>
       <c r="B90">
@@ -2622,7 +2622,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Cake (2015)</t>
+          <t xml:space="preserve">Cake </t>
         </is>
       </c>
       <c r="B91">
@@ -2647,7 +2647,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Into the Woods (2014)</t>
+          <t xml:space="preserve">Into the Woods </t>
         </is>
       </c>
       <c r="B92">
@@ -2672,7 +2672,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>It Follows (2015)</t>
+          <t xml:space="preserve">It Follows </t>
         </is>
       </c>
       <c r="B93">
@@ -2697,7 +2697,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Inherent Vice (2014)</t>
+          <t xml:space="preserve">Inherent Vice </t>
         </is>
       </c>
       <c r="B94">
@@ -2722,7 +2722,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>A Most Violent Year (2014)</t>
+          <t xml:space="preserve">A Most Violent Year </t>
         </is>
       </c>
       <c r="B95">
@@ -2747,7 +2747,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>While We're Young (2015)</t>
+          <t xml:space="preserve">While We're Young </t>
         </is>
       </c>
       <c r="B96">
@@ -2772,7 +2772,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Clouds of Sils Maria (2015)</t>
+          <t xml:space="preserve">Clouds of Sils Maria </t>
         </is>
       </c>
       <c r="B97">
@@ -2797,7 +2797,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Magic Mike XXL (2015)</t>
+          <t xml:space="preserve">Magic Mike XXL </t>
         </is>
       </c>
       <c r="B98">
@@ -2822,7 +2822,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Home (2015)</t>
+          <t xml:space="preserve">Home </t>
         </is>
       </c>
       <c r="B99">
@@ -2847,7 +2847,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>The Wedding Ringer (2015)</t>
+          <t xml:space="preserve">The Wedding Ringer </t>
         </is>
       </c>
       <c r="B100">
@@ -2872,7 +2872,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Woman in Gold (2015)</t>
+          <t xml:space="preserve">Woman in Gold </t>
         </is>
       </c>
       <c r="B101">
@@ -2897,7 +2897,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Mission: Impossible â€“ Rogue Nation (2015)</t>
+          <t xml:space="preserve">Mission: Impossible â€“ Rogue Nation </t>
         </is>
       </c>
       <c r="B102">
@@ -2922,7 +2922,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Amy (2015)</t>
+          <t xml:space="preserve">Amy </t>
         </is>
       </c>
       <c r="B103">
@@ -2947,7 +2947,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Jurassic World (2015)</t>
+          <t xml:space="preserve">Jurassic World </t>
         </is>
       </c>
       <c r="B104">
@@ -2972,7 +2972,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Minions (2015)</t>
+          <t xml:space="preserve">Minions </t>
         </is>
       </c>
       <c r="B105">
@@ -2997,7 +2997,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Paul Blart: Mall Cop 2 (2015)</t>
+          <t xml:space="preserve">Paul Blart: Mall Cop 2 </t>
         </is>
       </c>
       <c r="B106">
@@ -3022,7 +3022,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>The Longest Ride (2015)</t>
+          <t xml:space="preserve">The Longest Ride </t>
         </is>
       </c>
       <c r="B107">
@@ -3047,7 +3047,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>The Lazarus Effect (2015)</t>
+          <t xml:space="preserve">The Lazarus Effect </t>
         </is>
       </c>
       <c r="B108">
@@ -3072,7 +3072,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>The Woman In Black 2 Angel of Death (2015)</t>
+          <t xml:space="preserve">The Woman In Black 2 Angel of Death </t>
         </is>
       </c>
       <c r="B109">
@@ -3097,7 +3097,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Danny Collins (2015)</t>
+          <t xml:space="preserve">Danny Collins </t>
         </is>
       </c>
       <c r="B110">
@@ -3122,7 +3122,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Inside Out (2015)</t>
+          <t xml:space="preserve">Inside Out </t>
         </is>
       </c>
       <c r="B111">
@@ -3147,7 +3147,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Mr. Holmes (2015)</t>
+          <t xml:space="preserve">Mr. Holmes </t>
         </is>
       </c>
       <c r="B112">
@@ -3172,7 +3172,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>'71 (2015)</t>
+          <t xml:space="preserve">'71 </t>
         </is>
       </c>
       <c r="B113">
@@ -3197,7 +3197,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Two Days, One Night (2014)</t>
+          <t xml:space="preserve">Two Days, One Night </t>
         </is>
       </c>
       <c r="B114">

</xml_diff>